<commit_message>
Refactor timetable generation to improve formatting and readability by adding line breaks in activity descriptions. Update room mappings in CSV files for camps A and B. Remove outdated student timetable files to streamline resources.
</commit_message>
<xml_diff>
--- a/input/cello-campA-time-table.xlsx
+++ b/input/cello-campA-time-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A519C40-6754-484A-A74C-4F7A4ED48CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3778E08-F108-4655-901A-C79C1AFED730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="5" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
   </bookViews>
@@ -115,46 +115,12 @@
 (Room Sivan)</t>
   </si>
   <si>
-    <t>C3  Rehearsal with pianist
-(Room Queena)</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1 Rehearsal with pianist
-(Room Queena) </t>
-  </si>
-  <si>
-    <t>C2  Rehearsal with pianist
-(Room Queena)</t>
-  </si>
-  <si>
-    <t>C5   Rehearsal with pianist 
-(Room Queena)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6   Rehearsal with pianist
 (Room Queena) </t>
   </si>
   <si>
     <t>C4 Rehearsal with pianist
 (Room Queena)</t>
-  </si>
-  <si>
-    <t>C2 Lesson with Tomasz SKWERES &amp; pianist</t>
-  </si>
-  <si>
-    <t>C3 Lesson with Tomasz SKWERES &amp; pianist</t>
-  </si>
-  <si>
-    <t>C1 Lesson with Tomasz SKWERES &amp; pianist</t>
-  </si>
-  <si>
-    <t>C4  Lesson with Tomasz SKWERES &amp; pianist</t>
-  </si>
-  <si>
-    <t>C5  Lesson with Tomasz SKWERES &amp; pianist</t>
-  </si>
-  <si>
-    <t>C6  Lesson with Tomasz SKWERES &amp; pianist</t>
   </si>
   <si>
     <t>Group 4
@@ -205,12 +171,46 @@
     <t>Tomasz SKWERES</t>
   </si>
   <si>
-    <t>Cello Regulation &amp; Maintance Class
+    <t>Group 7
+(Room Gwyneth)</t>
+  </si>
+  <si>
+    <t>Cello Regulation / Maintance Workshop
 (Room TanCong)</t>
   </si>
   <si>
-    <t>Group 7
-(Room Gwyneth)</t>
+    <t>C5 Rehearsal with pianist 
+(Room Queena)</t>
+  </si>
+  <si>
+    <t>C2 Private Lesson with Tomasz SKWERES &amp; pianist</t>
+  </si>
+  <si>
+    <t>C3 Private Lesson with Tomasz SKWERES &amp; pianist</t>
+  </si>
+  <si>
+    <t>C1 Private Lesson with Tomasz SKWERES &amp; pianist</t>
+  </si>
+  <si>
+    <t>C4 Private Lesson with Tomasz SKWERES &amp; pianist</t>
+  </si>
+  <si>
+    <t>C5 Private Lesson with Tomasz SKWERES &amp; pianist</t>
+  </si>
+  <si>
+    <t>C6 Private Lesson with Tomasz SKWERES &amp; pianist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6 Rehearsal with pianist
+(Room Queena) </t>
+  </si>
+  <si>
+    <t>C3 Rehearsal with pianist
+(Room Queena)</t>
+  </si>
+  <si>
+    <t>C2 Rehearsal with pianist
+(Room Queena)</t>
   </si>
 </sst>
 </file>
@@ -298,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -495,12 +495,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,11 +553,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -560,42 +622,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -624,34 +658,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1013,7 +1043,7 @@
   <dimension ref="A1:G991"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="G23" sqref="G23:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -1024,18 +1054,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1048,68 +1078,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1119,7 +1149,7 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="31"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -1130,7 +1160,7 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="31"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1141,7 +1171,7 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="32"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -1150,22 +1180,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1206,68 +1236,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1308,108 +1338,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="33"/>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="28"/>
+      <c r="E27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -1426,10 +1456,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -2465,24 +2495,6 @@
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="B15:G18"/>
     <mergeCell ref="B3:G6"/>
@@ -2499,6 +2511,24 @@
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2509,7 +2539,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F30"/>
+      <selection activeCell="G23" sqref="G23:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -2520,18 +2550,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2544,68 +2574,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2614,7 +2644,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -2625,7 +2655,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="31"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -2636,7 +2666,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="32"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -2646,22 +2676,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2670,7 +2700,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="31"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -2681,7 +2711,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -2692,7 +2722,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2702,68 +2732,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2772,9 +2802,9 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
@@ -2783,9 +2813,9 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="52"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
@@ -2794,9 +2824,9 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
@@ -2804,108 +2834,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="33"/>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="28"/>
+      <c r="E27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2921,10 +2951,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -3962,6 +3992,32 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="E27:E30"/>
@@ -3970,32 +4026,6 @@
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4006,7 +4036,7 @@
   <dimension ref="A1:G989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F30"/>
+      <selection activeCell="E27" sqref="E27:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -4017,18 +4047,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -4039,68 +4069,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
+      <c r="B3" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4141,22 +4171,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4197,68 +4227,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4299,108 +4329,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="33"/>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="28"/>
+      <c r="E27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -4416,10 +4446,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -5442,20 +5472,13 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="B15:G18"/>
     <mergeCell ref="E11:E14"/>
@@ -5469,13 +5492,20 @@
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5486,7 +5516,7 @@
   <dimension ref="A1:G989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F30"/>
+      <selection activeCell="G23" sqref="G23:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -5497,18 +5527,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -5519,68 +5549,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5589,7 +5619,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -5600,7 +5630,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="31"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -5611,7 +5641,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="32"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -5621,22 +5651,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5645,7 +5675,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="31"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -5656,7 +5686,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -5667,7 +5697,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -5677,68 +5707,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="13" t="s">
+      <c r="C19" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5747,7 +5777,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="31"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
@@ -5758,7 +5788,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="31"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -5769,7 +5799,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="32"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -5779,108 +5809,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="33"/>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="28"/>
+      <c r="E27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -5896,10 +5926,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -6920,20 +6950,13 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="G11:G14"/>
@@ -6947,13 +6970,20 @@
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6964,7 +6994,7 @@
   <dimension ref="A1:F989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F30"/>
+      <selection activeCell="B15" sqref="B15:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -6976,18 +7006,18 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -6997,143 +7027,143 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
+      <c r="B7" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="55"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
@@ -7143,7 +7173,7 @@
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="55"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="56"/>
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
@@ -7153,153 +7183,153 @@
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
+      <c r="B19" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>34</v>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>48</v>
+      <c r="E27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
@@ -7313,10 +7343,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -8330,12 +8360,6 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
     <mergeCell ref="B19:F22"/>
     <mergeCell ref="B15:F18"/>
     <mergeCell ref="B7:F14"/>
@@ -8346,6 +8370,12 @@
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8353,10 +8383,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05693FB8-2279-484C-82DF-49EA93A50CE5}">
-  <dimension ref="A1:C989"/>
+  <dimension ref="A1:B987"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -8365,334 +8395,333 @@
     <col min="2" max="2" width="39.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="B3" s="60"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.4375</v>
+      </c>
+      <c r="B4" s="60"/>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="B5" s="59"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.44791666666666702</v>
+      </c>
+      <c r="B5" s="60"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
-        <v>0.4375</v>
-      </c>
-      <c r="B6" s="59"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
-        <v>0.44791666666666702</v>
-      </c>
-      <c r="B7" s="59"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.46875</v>
+      </c>
+      <c r="B7" s="62"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="B8" s="62"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
-        <v>0.46875</v>
-      </c>
-      <c r="B9" s="61"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="B9" s="62"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
-        <v>0.47916666666666702</v>
-      </c>
-      <c r="B10" s="61"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="62"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
-        <v>0.48958333333333298</v>
-      </c>
-      <c r="B11" s="61"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="B11" s="62"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B12" s="61"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="B12" s="62"/>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
-        <v>0.51041666666666696</v>
-      </c>
-      <c r="B13" s="61"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.53125</v>
+      </c>
+      <c r="B13" s="62"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="B14" s="61"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="B15" s="61"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="B15" s="64"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="B16" s="62" t="s">
-        <v>2</v>
-      </c>
+        <v>0.5625</v>
+      </c>
+      <c r="B16" s="64"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
-        <v>0.55208333333333304</v>
-      </c>
-      <c r="B17" s="63"/>
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="B17" s="64"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
-        <v>0.5625</v>
-      </c>
-      <c r="B18" s="63"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B18" s="65"/>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
-        <v>0.57291666666666696</v>
-      </c>
-      <c r="B19" s="63"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0.59375</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="B20" s="64"/>
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
-        <v>0.59375</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>19</v>
-      </c>
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="B21" s="62"/>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="B22" s="61" t="s">
-        <v>3</v>
-      </c>
+        <v>0.625</v>
+      </c>
+      <c r="B22" s="62"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
-        <v>0.61458333333333304</v>
-      </c>
-      <c r="B23" s="61"/>
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="B23" s="62"/>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="B24" s="61"/>
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="B24" s="62"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
-        <v>0.63541666666666696</v>
-      </c>
-      <c r="B25" s="61"/>
+        <v>0.65625</v>
+      </c>
+      <c r="B25" s="62"/>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
-        <v>0.64583333333333304</v>
-      </c>
-      <c r="B26" s="61"/>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="B26" s="62" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="B27" s="61"/>
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="B27" s="62"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="B28" s="61" t="s">
-        <v>17</v>
-      </c>
+        <v>0.6875</v>
+      </c>
+      <c r="B28" s="62"/>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
-        <v>0.67708333333333304</v>
-      </c>
-      <c r="B29" s="61"/>
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="B29" s="61" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
-        <v>0.6875</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="B30" s="61"/>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
-        <v>0.69791666666666696</v>
-      </c>
-      <c r="B31" s="60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.718749999999999</v>
+      </c>
+      <c r="B31" s="61"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="B32" s="60"/>
+        <v>0.72916666666666496</v>
+      </c>
+      <c r="B32" s="60" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
-        <v>0.718749999999999</v>
+        <v>0.73958333333333104</v>
       </c>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
-        <v>0.72916666666666496</v>
-      </c>
-      <c r="B34" s="59" t="s">
-        <v>12</v>
-      </c>
+        <v>0.749999999999997</v>
+      </c>
+      <c r="B34" s="60"/>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
-        <v>0.73958333333333104</v>
-      </c>
-      <c r="B35" s="59"/>
+        <v>0.76041666666666297</v>
+      </c>
+      <c r="B35" s="60"/>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
-        <v>0.749999999999997</v>
-      </c>
-      <c r="B36" s="59"/>
+        <v>0.77083333333332904</v>
+      </c>
+      <c r="B36" s="66" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
-        <v>0.76041666666666297</v>
-      </c>
-      <c r="B37" s="59"/>
+        <v>0.781249999999996</v>
+      </c>
+      <c r="B37" s="66"/>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
-        <v>0.77083333333332904</v>
-      </c>
-      <c r="B38" s="65" t="s">
-        <v>4</v>
-      </c>
+        <v>0.79166666666666297</v>
+      </c>
+      <c r="B38" s="66"/>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
-        <v>0.781249999999996</v>
-      </c>
-      <c r="B39" s="65"/>
+        <v>0.80208333333333004</v>
+      </c>
+      <c r="B39" s="66"/>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
-        <v>0.79166666666666297</v>
-      </c>
-      <c r="B40" s="65"/>
+        <v>0.812499999999997</v>
+      </c>
+      <c r="B40" s="66"/>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
-        <v>0.80208333333333004</v>
-      </c>
-      <c r="B41" s="65"/>
+        <v>0.82291666666666397</v>
+      </c>
+      <c r="B41" s="60" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
-        <v>0.812499999999997</v>
-      </c>
-      <c r="B42" s="65"/>
+        <v>0.83333333333333104</v>
+      </c>
+      <c r="B42" s="60"/>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
-        <v>0.82291666666666397</v>
-      </c>
-      <c r="B43" s="59" t="s">
-        <v>40</v>
-      </c>
+        <v>0.843749999999998</v>
+      </c>
+      <c r="B43" s="60"/>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
-        <v>0.83333333333333104</v>
-      </c>
-      <c r="B44" s="59"/>
+        <v>0.85416666666666496</v>
+      </c>
+      <c r="B44" s="61" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
-        <v>0.843749999999998</v>
-      </c>
-      <c r="B45" s="59"/>
+        <v>0.86458333333333204</v>
+      </c>
+      <c r="B45" s="61"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
-        <v>0.85416666666666496</v>
-      </c>
-      <c r="B46" s="60" t="s">
-        <v>41</v>
-      </c>
+        <v>0.874999999999999</v>
+      </c>
+      <c r="B46" s="61"/>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
-        <v>0.86458333333333204</v>
-      </c>
-      <c r="B47" s="60"/>
+        <v>0.88541666666666596</v>
+      </c>
+      <c r="B47" s="61"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
-        <v>0.874999999999999</v>
-      </c>
-      <c r="B48" s="60"/>
+        <v>0.89583333333333304</v>
+      </c>
+      <c r="B48" s="61"/>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
-        <v>0.88541666666666596</v>
-      </c>
-      <c r="B49" s="60"/>
+        <v>0.90625</v>
+      </c>
+      <c r="B49" s="61"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
-        <v>0.89583333333333304</v>
-      </c>
-      <c r="B50" s="60"/>
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="B50" s="61"/>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="1">
-        <v>0.90625</v>
-      </c>
-      <c r="B51" s="60"/>
+      <c r="B51" s="9"/>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="1">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="B52" s="60"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="9"/>
@@ -8709,12 +8738,8 @@
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="9"/>
     </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="9"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="9"/>
-    </row>
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9643,20 +9668,18 @@
     <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor timetable generation to ensure room information is consistently formatted on separate lines. Update room mappings in CSV files for camps A and B to correct room assignments. Replace outdated student timetable files to maintain resource accuracy.
</commit_message>
<xml_diff>
--- a/input/cello-campA-time-table.xlsx
+++ b/input/cello-campA-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3778E08-F108-4655-901A-C79C1AFED730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19AE87A-5E80-45FC-B8EB-A29950613E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="5" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="51">
   <si>
     <t xml:space="preserve">Faculty Rehearsal </t>
   </si>
@@ -175,10 +175,6 @@
 (Room Gwyneth)</t>
   </si>
   <si>
-    <t>Cello Regulation / Maintance Workshop
-(Room TanCong)</t>
-  </si>
-  <si>
     <t>C5 Rehearsal with pianist 
 (Room Queena)</t>
   </si>
@@ -211,6 +207,18 @@
   <si>
     <t>C2 Rehearsal with pianist
 (Room Queena)</t>
+  </si>
+  <si>
+    <t>Group 2, 5, 7, 9 Acting Class
+(Room Acting Class)</t>
+  </si>
+  <si>
+    <t>Group 1, 3, 4, 6, 8 Acting Class
+(Room Acting Class)</t>
+  </si>
+  <si>
+    <t>Cello Regulation / Maintenance Workshop
+(Room TanCong)</t>
   </si>
 </sst>
 </file>
@@ -553,42 +561,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -621,6 +598,43 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -666,17 +680,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1042,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BB261C-9115-4448-A297-AED1A944CF35}">
   <dimension ref="A1:G991"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:G26"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -1078,68 +1086,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1149,7 +1157,7 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="19"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -1160,7 +1168,7 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="19"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1171,7 +1179,7 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -1180,22 +1188,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="28" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1236,68 +1244,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="26" t="s">
+      <c r="D19" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1338,108 +1346,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="23" t="s">
+      <c r="D23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="21"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="D27" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="21"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -1456,10 +1464,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -2495,6 +2503,24 @@
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="B15:G18"/>
     <mergeCell ref="B3:G6"/>
@@ -2511,24 +2537,6 @@
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2538,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C31122-41FF-4E46-ACED-14E27AF0BAE7}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:G26"/>
+    <sheetView topLeftCell="A18" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -2574,68 +2582,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="C7" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2644,7 +2652,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="19"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -2655,7 +2663,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -2666,7 +2674,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="20"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -2676,22 +2684,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="28" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2700,7 +2708,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="19"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -2711,7 +2719,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="19"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -2722,7 +2730,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="19"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2732,68 +2740,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="50" t="s">
+      <c r="C19" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2802,9 +2810,9 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="52"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="54"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
@@ -2813,9 +2821,9 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="52"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="54"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
@@ -2824,9 +2832,9 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="53"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="55"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
@@ -2834,108 +2842,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="23" t="s">
+      <c r="D23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="21"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="D27" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="21"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2951,10 +2959,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -3992,32 +4000,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="E27:E30"/>
@@ -4026,6 +4008,32 @@
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4036,7 +4044,7 @@
   <dimension ref="A1:G989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E30"/>
+      <selection activeCell="E11" sqref="E11:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -4069,68 +4077,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
+      <c r="B3" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4171,22 +4179,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="28" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4227,68 +4235,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4329,108 +4337,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="23" t="s">
+      <c r="D23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="21"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="D27" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="21"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -4446,10 +4454,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -5472,13 +5480,20 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="B15:G18"/>
     <mergeCell ref="E11:E14"/>
@@ -5492,20 +5507,13 @@
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5516,7 +5524,7 @@
   <dimension ref="A1:G989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:G26"/>
+      <selection activeCell="D27" sqref="D27:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -5549,68 +5557,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="C7" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5619,7 +5627,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="19"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -5630,7 +5638,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -5641,7 +5649,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="20"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -5651,22 +5659,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5675,7 +5683,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="19"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -5686,7 +5694,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="19"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -5697,7 +5705,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="19"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -5707,68 +5715,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="26" t="s">
+      <c r="C19" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5777,7 +5785,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="19"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
@@ -5788,7 +5796,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="19"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -5799,7 +5807,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="20"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -5809,108 +5817,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="23" t="s">
+      <c r="D23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="21"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="D27" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="21"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -5926,10 +5934,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -6950,13 +6958,20 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="G11:G14"/>
@@ -6970,20 +6985,13 @@
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7027,43 +7035,43 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
@@ -7151,43 +7159,43 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
@@ -7235,19 +7243,19 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="33" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7255,49 +7263,49 @@
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="33" t="s">
         <v>37</v>
       </c>
     </row>
@@ -7305,31 +7313,31 @@
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
@@ -7343,10 +7351,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -8360,6 +8368,12 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
     <mergeCell ref="B19:F22"/>
     <mergeCell ref="B15:F18"/>
     <mergeCell ref="B7:F14"/>
@@ -8370,12 +8384,6 @@
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="F23:F26"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8385,7 +8393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05693FB8-2279-484C-82DF-49EA93A50CE5}">
   <dimension ref="A1:B987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement room mapping functionality in timetable generation, allowing for teacher-to-room assignments based on CSV input. Enhance activity formatting by including room numbers for specific MasterClass activities and adjusting header styles for improved readability. Update room mappings in CSV files for accuracy and remove outdated student and teacher timetable files to streamline resources.
</commit_message>
<xml_diff>
--- a/input/cello-campA-time-table.xlsx
+++ b/input/cello-campA-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19AE87A-5E80-45FC-B8EB-A29950613E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1110F04-CB3D-4817-9C0D-C8D98B8F97DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="5" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="2" r:id="rId1"/>
@@ -561,11 +561,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -598,43 +629,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,11 +674,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1050,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BB261C-9115-4448-A297-AED1A944CF35}">
   <dimension ref="A1:G991"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:D30"/>
     </sheetView>
   </sheetViews>
@@ -1086,68 +1086,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="31"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="31"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="32"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -1188,22 +1188,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1244,68 +1244,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1346,108 +1346,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -1464,10 +1464,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -2503,24 +2503,6 @@
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="B15:G18"/>
     <mergeCell ref="B3:G6"/>
@@ -2537,6 +2519,24 @@
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2582,68 +2582,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -2663,7 +2663,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="31"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -2674,7 +2674,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="32"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -2684,22 +2684,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2708,7 +2708,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="31"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -2719,7 +2719,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -2730,7 +2730,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2740,68 +2740,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="45"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2810,9 +2810,9 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="54"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
@@ -2821,9 +2821,9 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="54"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="52"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
@@ -2832,9 +2832,9 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="55"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
@@ -2842,108 +2842,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2959,10 +2959,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -4000,6 +4000,32 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="E27:E30"/>
@@ -4008,32 +4034,6 @@
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4077,68 +4077,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4179,22 +4179,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4235,68 +4235,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4337,108 +4337,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -4454,10 +4454,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -5480,20 +5480,13 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="B15:G18"/>
     <mergeCell ref="E11:E14"/>
@@ -5507,13 +5500,20 @@
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5557,68 +5557,68 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -5638,7 +5638,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="31"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -5649,7 +5649,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="32"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -5659,22 +5659,22 @@
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5683,7 +5683,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="31"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -5694,7 +5694,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -5705,7 +5705,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -5715,68 +5715,68 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5785,7 +5785,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="31"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
@@ -5796,7 +5796,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="31"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -5807,7 +5807,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="32"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -5817,108 +5817,108 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -5934,10 +5934,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -6958,20 +6958,13 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="G11:G14"/>
@@ -6985,13 +6978,20 @@
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7035,43 +7035,43 @@
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
@@ -7159,43 +7159,43 @@
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
@@ -7243,19 +7243,19 @@
       <c r="A23" s="1">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="23" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7263,49 +7263,49 @@
       <c r="A24" s="1">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -7313,31 +7313,31 @@
       <c r="A28" s="1">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
@@ -7351,10 +7351,10 @@
       <c r="A32" s="1">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
@@ -8368,12 +8368,6 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
     <mergeCell ref="B19:F22"/>
     <mergeCell ref="B15:F18"/>
     <mergeCell ref="B7:F14"/>
@@ -8384,6 +8378,12 @@
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8393,7 +8393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05693FB8-2279-484C-82DF-49EA93A50CE5}">
   <dimension ref="A1:B987"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update time tables for cello and flute camps A and B, and harp camps A and B to reflect recent changes in scheduling data, ensuring accuracy and consistency across all camp activities.
</commit_message>
<xml_diff>
--- a/input/cello-campA-time-table.xlsx
+++ b/input/cello-campA-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1110F04-CB3D-4817-9C0D-C8D98B8F97DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E17680-224C-422A-AC4E-FEB3D3744D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="5" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="4" xr2:uid="{F2BB48B4-7D7C-49F7-8C87-D227621DCE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="2" r:id="rId1"/>
@@ -131,10 +131,6 @@
 (Room Ivy)</t>
   </si>
   <si>
-    <t>Cello MasterClass
-(Room Tomasz)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Time </t>
   </si>
   <si>
@@ -219,6 +215,10 @@
   <si>
     <t>Cello Regulation / Maintenance Workshop
 (Room TanCong)</t>
+  </si>
+  <si>
+    <t>Cello MasterClass by Tomasz SWKERES
+(Room Tomasz)</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:G991"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+      <selection activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -1062,18 +1062,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1087,7 +1087,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -1139,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>9</v>
@@ -1297,7 +1297,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>5</v>
@@ -1353,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>21</v>
@@ -1407,13 +1407,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="21"/>
     </row>
@@ -1535,17 +1535,13 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>0.79166666666666197</v>
-      </c>
+      <c r="A39" s="1"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>0.80208333333332804</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -2547,7 +2543,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView topLeftCell="A18" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+      <selection activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -2558,18 +2554,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2583,7 +2579,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2632,7 +2628,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>5</v>
@@ -2688,7 +2684,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>5</v>
@@ -2790,7 +2786,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>10</v>
@@ -2849,7 +2845,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>21</v>
@@ -2903,13 +2899,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="21"/>
     </row>
@@ -3023,16 +3019,12 @@
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>0.79166666666666197</v>
-      </c>
+      <c r="A39" s="1"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>0.80208333333332804</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
@@ -4044,7 +4036,7 @@
   <dimension ref="A1:G989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E14"/>
+      <selection activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -4055,18 +4047,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -4078,7 +4070,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -4130,7 +4122,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>7</v>
@@ -4186,7 +4178,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>7</v>
@@ -4344,7 +4336,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>21</v>
@@ -4398,13 +4390,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="21"/>
     </row>
@@ -4518,14 +4510,10 @@
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>0.79166666666666197</v>
-      </c>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>0.80208333333332804</v>
-      </c>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
@@ -5524,7 +5512,7 @@
   <dimension ref="A1:G989"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+      <selection activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -5535,18 +5523,18 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -5558,7 +5546,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -5607,7 +5595,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>10</v>
@@ -5663,7 +5651,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>10</v>
@@ -5765,7 +5753,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>7</v>
@@ -5824,7 +5812,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>21</v>
@@ -5878,13 +5866,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="21"/>
     </row>
@@ -5998,14 +5986,10 @@
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>0.79166666666666197</v>
-      </c>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>0.80208333333332804</v>
-      </c>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7001,8 +6985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320C05D6-4C9A-A343-B543-784FF534AB03}">
   <dimension ref="A1:F989"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:F18"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -7014,18 +6998,18 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -7078,7 +7062,7 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="59"/>
@@ -7202,7 +7186,7 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
@@ -7250,7 +7234,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>21</v>
@@ -7300,13 +7284,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -7408,14 +7392,10 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>0.79166666666666197</v>
-      </c>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>0.80208333333332804</v>
-      </c>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8393,7 +8373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05693FB8-2279-484C-82DF-49EA93A50CE5}">
   <dimension ref="A1:B987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -8405,7 +8385,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -8666,7 +8646,7 @@
         <v>0.82291666666666397</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -8686,7 +8666,7 @@
         <v>0.85416666666666496</v>
       </c>
       <c r="B44" s="61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>